<commit_message>
Now view log history
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kieran\OneDrive\School\High School\AOS\Science\Senior Research Project\Inventory\Python\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_5CBFB0FCDA426F7E1B502D4CE571B0B0D710212D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ECDD537B-BB4C-403C-AB8E-D60369C21667}"/>
   <bookViews>
-    <workbookView xWindow="2562" yWindow="2562" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
     <sheet name="1" sheetId="2" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -63,13 +59,25 @@
   </si>
   <si>
     <t>11:13AM</t>
+  </si>
+  <si>
+    <t>Varun</t>
+  </si>
+  <si>
+    <t>01:50PM</t>
+  </si>
+  <si>
+    <t>02:00PM</t>
+  </si>
+  <si>
+    <t>12/3/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,14 +140,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -186,7 +186,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,27 +218,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,24 +252,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,14 +427,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -516,16 +480,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="A3:F4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -563,6 +525,92 @@
       </c>
       <c r="F2" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds another item and now doesn't display item not movable when no item is selected
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -11,13 +11,16 @@
     <sheet name="1" sheetId="2" r:id="rId2"/>
     <sheet name="2" sheetId="3" r:id="rId3"/>
     <sheet name="3" sheetId="4" r:id="rId4"/>
+    <sheet name="4" sheetId="5" r:id="rId5"/>
+    <sheet name="5" sheetId="6" r:id="rId6"/>
+    <sheet name="6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -43,19 +46,10 @@
     <t>JP</t>
   </si>
   <si>
-    <t>stupid</t>
-  </si>
-  <si>
     <t>Mr. T</t>
   </si>
   <si>
-    <t>faggot</t>
-  </si>
-  <si>
     <t>Crowe</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>02:11PM</t>
@@ -449,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,19 +474,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -500,39 +494,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -573,19 +547,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -623,22 +597,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -677,4 +651,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Now changes the room based on the log and autofills that room on checkout
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -46,6 +46,9 @@
     <t>JP</t>
   </si>
   <si>
+    <t>Joe</t>
+  </si>
+  <si>
     <t>Mr. T</t>
   </si>
   <si>
@@ -58,18 +61,27 @@
     <t>01:00PM</t>
   </si>
   <si>
+    <t>03:21PM</t>
+  </si>
+  <si>
     <t>02:15PM</t>
   </si>
   <si>
     <t>01:05PM</t>
   </si>
   <si>
+    <t>01:30AM</t>
+  </si>
+  <si>
     <t>12/2/2019</t>
   </si>
   <si>
     <t>12/5/2019</t>
   </si>
   <si>
+    <t>12/7/2019</t>
+  </si>
+  <si>
     <t>11:10AM</t>
   </si>
   <si>
@@ -86,6 +98,39 @@
   </si>
   <si>
     <t>12/3/2019</t>
+  </si>
+  <si>
+    <t>alka</t>
+  </si>
+  <si>
+    <t>03:37PM</t>
+  </si>
+  <si>
+    <t>12:37AM</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>rwyn</t>
+  </si>
+  <si>
+    <t>wer</t>
+  </si>
+  <si>
+    <t>Profitt</t>
+  </si>
+  <si>
+    <t>sgn</t>
+  </si>
+  <si>
+    <t>02:27PM</t>
+  </si>
+  <si>
+    <t>01:29PM</t>
+  </si>
+  <si>
+    <t>11:25PM</t>
   </si>
 </sst>
 </file>
@@ -443,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,19 +519,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -494,19 +539,79 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -547,19 +652,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -597,22 +702,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +760,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -679,6 +784,26 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +846,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -747,6 +872,46 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>